<commit_message>
modificando padrões para dados sensiveis
</commit_message>
<xml_diff>
--- a/Tabela CEMIG.xlsx
+++ b/Tabela CEMIG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilbe\Desktop\PI_ADTEC_IA_LGPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6971A442-225E-4CDA-8636-88925AA95914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94AD6DD-DFE2-41F6-AD10-54BA5FC0CBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crie um arquivo excel com dados" sheetId="1" r:id="rId1"/>
@@ -926,7 +926,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>